<commit_message>
19 and 20 LeetCode done
</commit_message>
<xml_diff>
--- a/Yandex_learning/interview/Задача.xlsx
+++ b/Yandex_learning/interview/Задача.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shoma\Documents\Learning\Yandex_learning\interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436B4840-14E2-4289-AAE6-A11539E39931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0089091-72A2-4399-89A3-5909245A95A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{9F686658-B38A-AF43-87BC-8862ADFA90CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
   <si>
     <t>Line Reflection</t>
   </si>
@@ -653,7 +653,7 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -974,6 +974,9 @@
       <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="G19" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1">
@@ -984,6 +987,12 @@
       </c>
       <c r="C20" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:8">

</xml_diff>

<commit_message>
32 33 leetcode done
</commit_message>
<xml_diff>
--- a/Yandex_learning/interview/Задача.xlsx
+++ b/Yandex_learning/interview/Задача.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shoma\Documents\Learning\Yandex_learning\interview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shoma/Learning/Yandex_learning/interview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86C429C-7BA8-41D2-ABCF-879C3B95206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3430C8-D7F8-CC46-914A-A240E75FE930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{9F686658-B38A-AF43-87BC-8862ADFA90CD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23980" windowHeight="19920" xr2:uid="{9F686658-B38A-AF43-87BC-8862ADFA90CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
     <t>Line Reflection</t>
   </si>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t>Разобрано</t>
-  </si>
-  <si>
-    <t>50/50, можно лучше</t>
   </si>
   <si>
     <t>Пропущено</t>
@@ -668,11 +665,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F341B8F-6337-7643-A497-1C0AC0EBA6FD}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1">
@@ -943,7 +940,7 @@
         <v>70</v>
       </c>
       <c r="I16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1118,7 +1115,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1152,10 +1149,10 @@
         <v>69</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1185,6 +1182,12 @@
       <c r="C31" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="G31" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
@@ -1196,8 +1199,14 @@
       <c r="C32" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -1207,8 +1216,14 @@
       <c r="C33" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="G33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -1219,7 +1234,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -1230,7 +1245,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -1241,7 +1256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -1252,7 +1267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -1263,7 +1278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -1274,7 +1289,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -1285,7 +1300,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1296,7 +1311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -1307,7 +1322,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -1318,7 +1333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -1340,7 +1355,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -1351,7 +1366,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -1362,7 +1377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>48</v>
       </c>

</xml_diff>